<commit_message>
Revert "Merge branch 'master' of https://github.com/michjens/Kino-XP"
This reverts commit 13a9a633b3b8ebfa1102fc75d1ffdce682bf3524, reversing
changes made to 474a245446b0ed1a643c2ab69f2959ecbab1e8e5.
</commit_message>
<xml_diff>
--- a/Rapport/Burndown Chart Kino XP.xlsx
+++ b/Rapport/Burndown Chart Kino XP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Casper\Desktop\Kino-XP\Rapport\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A22431B-EC63-4532-A797-2C6E93CA0891}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFA48F1A-AB67-4374-A5B5-D4FDA0980A9E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6975" yWindow="0" windowWidth="27405" windowHeight="12810" xr2:uid="{CADBAEDD-29BA-4A58-BDD9-E1DB6333F0B2}"/>
+    <workbookView xWindow="5580" yWindow="0" windowWidth="27405" windowHeight="12810" xr2:uid="{CADBAEDD-29BA-4A58-BDD9-E1DB6333F0B2}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
   <si>
     <t>Iteration 1</t>
   </si>
@@ -114,18 +114,6 @@
   </si>
   <si>
     <t>Consumable hours iteration 1:</t>
-  </si>
-  <si>
-    <t>Used day 2 (t)</t>
-  </si>
-  <si>
-    <t>Tilføj status til sæder</t>
-  </si>
-  <si>
-    <t>CSS forside</t>
-  </si>
-  <si>
-    <t>Separat header</t>
   </si>
 </sst>
 </file>
@@ -803,450 +791,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="da-DK"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="da-DK"/>
-              <a:t>Iteration 2</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="da-DK"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Ark1'!$F$17</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Estimated left</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>'Ark1'!$F$18:$F$20</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>36</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-925F-47D4-9DD5-AC0FCA0397AA}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Ark1'!$G$17</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Actual left</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>'Ark1'!$G$18:$G$20</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>36</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>19.09</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>7.59</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-925F-47D4-9DD5-AC0FCA0397AA}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="163309807"/>
-        <c:axId val="160242399"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="163309807"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="da-DK"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="160242399"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="160242399"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="da-DK"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="163309807"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="da-DK"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="da-DK"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1449,509 +994,6 @@
       <a:solidFill>
         <a:schemeClr val="phClr"/>
       </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2340,42 +1382,6 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>604837</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>300037</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Diagram 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BC7AD9F5-4498-482E-B2D6-2BA735CBCC26}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2681,10 +1687,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E23570A-1FA5-4B45-ADC2-3588A643C865}">
-  <dimension ref="A1:H27"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+      <selection activeCell="F17" sqref="F17:G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2941,14 +1947,12 @@
       <c r="C16" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="10" t="s">
-        <v>28</v>
-      </c>
+      <c r="D16" s="10"/>
       <c r="E16" s="10" t="s">
         <v>26</v>
       </c>
       <c r="F16">
-        <v>36</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -2961,9 +1965,6 @@
       <c r="C17">
         <v>6</v>
       </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
       <c r="E17" s="1" t="s">
         <v>1</v>
       </c>
@@ -2984,17 +1985,14 @@
       <c r="C18">
         <v>3.25</v>
       </c>
-      <c r="D18">
-        <v>1.5</v>
-      </c>
       <c r="E18">
         <v>0</v>
       </c>
       <c r="F18">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="G18">
-        <v>36</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -3007,18 +2005,15 @@
       <c r="C19">
         <v>0.5</v>
       </c>
-      <c r="D19">
-        <v>1.5</v>
-      </c>
       <c r="E19">
         <v>1</v>
       </c>
       <c r="F19">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="G19">
-        <f>G18-SUM(C17:C26)</f>
-        <v>19.09</v>
+        <f>G18-SUM(C17:C23)</f>
+        <v>7.09</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -3031,19 +2026,6 @@
       <c r="C20">
         <v>1.5</v>
       </c>
-      <c r="D20">
-        <v>0</v>
-      </c>
-      <c r="E20">
-        <v>2</v>
-      </c>
-      <c r="F20">
-        <v>0</v>
-      </c>
-      <c r="G20">
-        <f>G19-SUM(D17:D26)</f>
-        <v>7.59</v>
-      </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
@@ -3055,9 +2037,6 @@
       <c r="C21">
         <v>2</v>
       </c>
-      <c r="D21">
-        <v>3</v>
-      </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
@@ -3069,9 +2048,6 @@
       <c r="C22">
         <v>0.66</v>
       </c>
-      <c r="D22">
-        <v>1</v>
-      </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
@@ -3083,67 +2059,18 @@
       <c r="C23">
         <v>3</v>
       </c>
-      <c r="D23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="B24">
-        <v>1</v>
-      </c>
-      <c r="C24">
-        <v>0</v>
-      </c>
-      <c r="D24">
-        <v>1</v>
-      </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="11" t="s">
-        <v>29</v>
+      <c r="A25" s="1" t="s">
+        <v>2</v>
       </c>
       <c r="B25">
-        <v>4</v>
+        <f>SUM(B17:B23)</f>
+        <v>21</v>
       </c>
       <c r="C25">
-        <v>0</v>
-      </c>
-      <c r="D25">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B26">
-        <v>1</v>
-      </c>
-      <c r="C26">
-        <v>0</v>
-      </c>
-      <c r="D26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B27">
-        <f>SUM(B17:B26)</f>
-        <v>27</v>
-      </c>
-      <c r="C27">
-        <f>SUM(C17:C26)</f>
+        <f>SUM(C17:C23)</f>
         <v>16.91</v>
-      </c>
-      <c r="D27">
-        <f>SUM(D17:D26)</f>
-        <v>11.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>